<commit_message>
Final changes for the practice
</commit_message>
<xml_diff>
--- a/Valores equipos/Merge.xlsx
+++ b/Valores equipos/Merge.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\ITESO (9 Noveno Semestre)\Ingeniería en Nanomateriales II\Práctica 4\Valores equipos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D65031B-6C19-497F-8D16-3E58165C7D7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B349DEC-05C1-489A-B539-741A61B930DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8EA125AB-A1D7-45F1-8CF2-96691AE2417F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8EA125AB-A1D7-45F1-8CF2-96691AE2417F}"/>
   </bookViews>
   <sheets>
-    <sheet name="K1" sheetId="1" r:id="rId1"/>
-    <sheet name="K2" sheetId="2" r:id="rId2"/>
+    <sheet name="K3" sheetId="3" r:id="rId1"/>
+    <sheet name="K1" sheetId="1" r:id="rId2"/>
+    <sheet name="K2" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'K3'!$A$2:$A$7</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'K3'!$B$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'K3'!$B$2:$B$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="26">
   <si>
     <t>Angle ($\theta$)</t>
   </si>
@@ -105,6 +111,12 @@
   <si>
     <t>conditions</t>
   </si>
+  <si>
+    <t>Espesor:</t>
+  </si>
+  <si>
+    <t>2.56nm</t>
+  </si>
 </sst>
 </file>
 
@@ -174,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -247,13 +259,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -318,6 +339,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,6 +359,2818 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'K3'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>R</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'K3'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'K3'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.3019529141675603</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.864156124969421</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5555622758888834</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5306656343117249</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8117588667223323</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.81906700245988</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0228-41D8-A4AF-712D9D02C887}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="532414072"/>
+        <c:axId val="532413432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="532414072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532413432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="532413432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532414072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'K3'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'K3'!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'K3'!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.70576926386386052</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95419867489843946</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2656207342363159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.685041436184749</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.6805985804508081</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.09441498174815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D333-44E6-BA59-18956975F2CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="532414072"/>
+        <c:axId val="532413432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="532414072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532413432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="532413432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532414072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Gráfica de espesor</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'K3'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ln ( 1+ R/K )</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'K3'!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>11.4737132456699</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8637033051562741</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.366201583152499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7434467956210979</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4142135623730949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2207745887614561</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'K3'!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.1415125880165466</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8079009159519337</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5259408066049391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4544700327834201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.86506679905380546</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61478499070787529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9DC3-4964-AEF5-AEA8A76C1199}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="532414072"/>
+        <c:axId val="532413432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="532414072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532413432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="532413432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="532414072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>109396</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114678</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1060010</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>141838</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2CA8685-891C-4E91-8F2A-520C994ECFCB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>414950</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>128257</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>15089</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>155417</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECF240E3-0FE3-4695-9341-5EF3353030CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>113168</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>105624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1063782</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>132784</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F0CCC83-BC27-4578-A734-808286E3826F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -633,6 +3469,224 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B097325-66B8-464C-A644-4E7EAC5A7DC5}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="101" workbookViewId="0">
+      <selection sqref="A1:K42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.5546875" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="24">
+        <v>5</v>
+      </c>
+      <c r="B2" s="24">
+        <v>0.70576926386386052</v>
+      </c>
+      <c r="C2" s="18">
+        <v>5.3019529141675603</v>
+      </c>
+      <c r="D2" s="24">
+        <f t="shared" ref="D2:D7" si="0">LN(1+C2/B2)</f>
+        <v>2.1415125880165466</v>
+      </c>
+      <c r="E2" s="24">
+        <v>11.4737132456699</v>
+      </c>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="24">
+        <v>15</v>
+      </c>
+      <c r="B3" s="24">
+        <v>0.95419867489843946</v>
+      </c>
+      <c r="C3" s="18">
+        <v>4.864156124969421</v>
+      </c>
+      <c r="D3" s="24">
+        <f t="shared" si="0"/>
+        <v>1.8079009159519337</v>
+      </c>
+      <c r="E3" s="24">
+        <v>3.8637033051562741</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="24">
+        <v>25</v>
+      </c>
+      <c r="B4" s="24">
+        <v>1.2656207342363159</v>
+      </c>
+      <c r="C4" s="18">
+        <v>4.5555622758888834</v>
+      </c>
+      <c r="D4" s="24">
+        <f t="shared" si="0"/>
+        <v>1.5259408066049391</v>
+      </c>
+      <c r="E4" s="24">
+        <v>2.366201583152499</v>
+      </c>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="24">
+        <v>35</v>
+      </c>
+      <c r="B5" s="24">
+        <v>1.685041436184749</v>
+      </c>
+      <c r="C5" s="18">
+        <v>5.5306656343117249</v>
+      </c>
+      <c r="D5" s="24">
+        <f t="shared" si="0"/>
+        <v>1.4544700327834201</v>
+      </c>
+      <c r="E5" s="24">
+        <v>1.7434467956210979</v>
+      </c>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="24">
+        <v>45</v>
+      </c>
+      <c r="B6" s="24">
+        <v>5.6805985804508081</v>
+      </c>
+      <c r="C6" s="18">
+        <v>7.8117588667223323</v>
+      </c>
+      <c r="D6" s="24">
+        <f t="shared" si="0"/>
+        <v>0.86506679905380546</v>
+      </c>
+      <c r="E6" s="24">
+        <v>1.4142135623730949</v>
+      </c>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="24">
+        <v>55</v>
+      </c>
+      <c r="B7" s="24">
+        <v>15.09441498174815</v>
+      </c>
+      <c r="C7" s="18">
+        <v>12.81906700245988</v>
+      </c>
+      <c r="D7" s="24">
+        <f t="shared" si="0"/>
+        <v>0.61478499070787529</v>
+      </c>
+      <c r="E7" s="24">
+        <v>1.2207745887614561</v>
+      </c>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K21" s="9"/>
+    </row>
+    <row r="22" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K24" s="9"/>
+    </row>
+    <row r="25" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="K25" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B94453-FEDE-4FB6-BF25-8648C740F96C}">
   <dimension ref="A1:M1048576"/>
   <sheetViews>
@@ -2239,11 +5293,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAA1FCE-7503-4F7B-A61E-A16ECCF796E0}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+    <sheetView zoomScale="101" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>

</xml_diff>